<commit_message>
- Fixed grammar issues. - Added DB.
</commit_message>
<xml_diff>
--- a/MedicalMasks.xlsx
+++ b/MedicalMasks.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feder\Documents\UiPath\MedicalMasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90422168-0318-4A77-8DE4-780B4AA5AC96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B4349E-8CB8-4F31-85BE-6C66D732CDA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="3360" windowWidth="20520" windowHeight="9000" xr2:uid="{4806D546-8CFD-4C5F-90A3-67386C377A3A}"/>
+    <workbookView xWindow="2520" yWindow="3360" windowWidth="20520" windowHeight="9000" xr2:uid="{4806D546-8CFD-4C5F-90A3-67386C377A3A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="7" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="17" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="99">
   <si>
     <t>Name</t>
   </si>
@@ -48,6 +48,21 @@
     <t>URL</t>
   </si>
   <si>
+    <t>[50 Pcs] 3-Ply Stylish Disposable Face Masks Non-Medical Surgical Earloop Cover</t>
+  </si>
+  <si>
+    <t>✅IN STOCK ✅SAME DAY HANDLING ✅FAST SHIPPING ✅HOT SALE!!</t>
+  </si>
+  <si>
+    <t>$27.99 to $28.99</t>
+  </si>
+  <si>
+    <t>From United States</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/50-Pcs-3-Ply-Stylish-Disposable-Face-Masks-Non-Medical-Surgical-Earloop-Cover/174343126809?hash=item2897a8ff19%3Ag%3Ac9UAAOSwxL1fBrfv&amp;LH_BIN=1</t>
+  </si>
+  <si>
     <t>10/20/50 Face Mask Mouth Cover Surgical MEDICAL Dental Disposable 3-PLY Earloop</t>
   </si>
   <si>
@@ -57,22 +72,19 @@
     <t>$7.95 to $4,240.89</t>
   </si>
   <si>
-    <t>From United States</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/10-20-50-Face-Mask-Mouth-Cover-Surgical-MEDICAL-Dental-Disposable-3-PLY-Earloop/193479410659?_trkparms=ispr%3D1&amp;hash=item2d0c4583e3%3Ag%3ABnsAAOSwKuleyaE4&amp;enc=AQAFAAACYBaobrjLl8XobRIiIML1V4Imu%2Fn%2BzU5L90Z278x5ickkfKe2vUidqHRg3XM2X2xOVCbCPmac8DIibqWJH0lp%2FMwgNTjECA6uBPtzM4v7lWBpiEiZdhMCwNqTbgK8oAK3%2Fvs8j1XCw1Cv1jIKDhXrARJAsTGk9BxYJPmEsSrZHW3LoKcuUcENhH43V5grXGwfFe7l4QMIVkv4lS2AcvR06aCa%2FcRiXBrV9QaGCvUy9eapT%2BENV22zqnl2nu7173oWaFiMITWD6W2xfj4MDuCTmEDiXPMpws7N%2F6EUeGBbyGBYtqGeVWv6a6oGJCbPdx%2F5s9y0Wuu%2Fhm%2BLK%2FGAlQ4HkGdJX0dvUu4na%2F2wB%2FJGUIsBmorj0stl7%2B%2BAWHRwfwZ3Y4YybXM4k8JxNTEWrNnxr3DGn77uVnh3LHQcSa0E2o3pz5ayrBdqMh0UJOVAIz4HwhlOwk1arHvpeNn7XFotEjnhm8agibtoRr5STfDobaWazCO%2BgU%2Fmgz9zhwv4A%2BYJfKCS3lYEmyt6orqy7bwkjy0llL5P%2BE%2F6dU79Y%2FY370PKHmFLNUA3293f18MxhdiSKeyzA%2FQpVrsBHEv8WxgpodiYcaobzDpawsLXXmW83avjf%2B1eem911bPj5ZFZVR5tSoSkoWWg7x%2FeyKT638DGTgae6tGhRzvmtFCUYYqYDGt3j1NZ3B90x09yEJQm3cQM5QJMuz9xN5ISqio5Yc3OTm3Sa%2FqVOk5XYAF0muTCuWebJSXYAvX%2BIgTUUqNYvwYX3V8jIUWnrDvJ52zL%2FnAaHU3PJUAWqBqn6zyZNQWv8vHZ&amp;checksum=193479410659b432771eb0044b8eb5eb88be336293dc&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>[50 Pcs] 3-Ply Stylish Disposable Face Masks Non-Medical Surgical Earloop Cover</t>
-  </si>
-  <si>
-    <t>✅IN STOCK ✅SAME DAY HANDLING ✅FAST SHIPPING ✅HOT SALE!!</t>
-  </si>
-  <si>
-    <t>$27.99 to $28.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50-Pcs-3-Ply-Stylish-Disposable-Face-Masks-Non-Medical-Surgical-Earloop-Cover/174343126809?hash=item2897a8ff19%3Ag%3Ac9UAAOSwxL1fBrfv&amp;LH_BIN=1</t>
+    <t>https://www.ebay.com/itm/10-20-50-Face-Mask-Mouth-Cover-Surgical-MEDICAL-Dental-Disposable-3-PLY-Earloop/193479410659?_trkparms=ispr%3D1&amp;hash=item2d0c4583e3%3Ag%3ABnsAAOSwKuleyaE4&amp;enc=AQAFAAACcBaobrjLl8XobRIiIML1V4Imu%2Fn%2BzU5L90Z278x5ickkfKe2vUidqHRg3XM2X2xOVCbCPmac8DIibqWJH0lp%2FMwgNTjECA6uBPtzM4v7lWBpiEiZdhMCwNqTbgK8oAK3%2Fvs8j1XCw1Cv1jIKDhXrARJAsTGk9BxYJPmEsSrZHW3LoKcuUcENhH43V5grXGwfFe7l4QMIVkv4lS2AcvR06aCa%2FcRiXBrV9QaGCvUy9eapT%2BENV22zqnl2nu7173oWaFiMITWD6W2xfj4MDuCTmEDiXPMpws7N%2F6EUeGBbyGBYtqGeVWv6a6oGJCbPdx%2F5s9y0Wuu%2Fhm%2BLK%2FGAlQ4HkGd%2BU4F%2BGUgdQguLnOgltwNcCTZIQx1J4bC5ZyYPSfPBpulBetDG1zQ%2Fxlso48LiyU%2B9vK%2FacPMqYodblVdB4JgopJ4MV83jYTGDsTk3cAon8%2BxI8voLTxUEusLKcAypJR2wGmFYEOIWgDrOBIBTy3h66g5kFkJ0g1b7U8vhIaPbyNY8wnnz8umE752R6BbxIivZ528jiZqNMR1enWvRLKKiN31nucMXmbtVDD%2Be12vtprhtdnnL6kbEHt15kBisxryokOQAGfQM4p73EoJdtVzsAUjpbcBtH1c%2Fg2UhktWyIdHcI%2FptYIU4AFhX75cS5i6KUnCBG%2FhDOg0KgDVIKn%2BmP9eb9H03SaVU9xXoOmGnLChTbYzkyr2jB8Qeid0xJQZJJmRzGbggwRdCjlxd0w4APslSJI3M6ZPXBwpiah7SLZpu3bXqwAAv3AfJ8Zb5A2IIAZwxalpq39IdTe%2FoS0vH%2F9%2F8erc9f4PUSG1BEx4jGA%3D%3D&amp;checksum=193479410659e3d4365e97684e009f553990af32581b&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>50/100 Face Mask Disposable 3-Ply Ear-loop Mouth Cover 3 Layer Filter Mask White</t>
+  </si>
+  <si>
+    <t>IN STOCK, USA FREE SHIPPING, SHIP OUT IN 1 BUSINESS DAY</t>
+  </si>
+  <si>
+    <t>$28.99 to $57.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/50-100-Face-Mask-Disposable-3-Ply-Ear-loop-Mouth-Cover-3-Layer-Filter-Mask-White/254593177423?hash=item3b46ef974f%3Ag%3A%7E5cAAOSwCV9e6fPt&amp;LH_BIN=1</t>
   </si>
   <si>
     <t>[White] 50/100 Pc 3-Ply Disposable Face Masks Non-Medical Surgical Earloop Cover</t>
@@ -87,18 +99,6 @@
     <t>https://www.ebay.com/itm/White-50-100-Pc-3-Ply-Disposable-Face-Masks-Non-Medical-Surgical-Earloop-Cover/153965253175?hash=item23d90b5237%3Ag%3AtaUAAOSw1Exe3uBZ&amp;LH_BIN=1</t>
   </si>
   <si>
-    <t>50/100 Face Mask Disposable 3-Ply Ear-loop Mouth Cover 3 Layer Filter Mask White</t>
-  </si>
-  <si>
-    <t>IN STOCK, USA FREE SHIPPING, SHIP OUT IN 1 BUSINESS DAY</t>
-  </si>
-  <si>
-    <t>$28.99 to $57.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50-100-Face-Mask-Disposable-3-Ply-Ear-loop-Mouth-Cover-3-Layer-Filter-Mask-White/254593177423?hash=item3b46ef974f%3Ag%3A%7E5cAAOSwCV9e6fPt&amp;LH_BIN=1</t>
-  </si>
-  <si>
     <t>50/100 PCS Face Mask 3-Ply Disposable Medical Masks Mouth cover shield USA</t>
   </si>
   <si>
@@ -111,6 +111,15 @@
     <t>https://www.ebay.com/itm/50-100-PCS-Face-Mask-3-Ply-Disposable-Medical-Masks-Mouth-cover-shield-USA/184291307042?hash=item2ae89e2e22%3Ag%3ArQ0AAOSwCTZe6tlW&amp;LH_BIN=1</t>
   </si>
   <si>
+    <t>50 PCS Face Mask Medical Surgical Disposable 3-Ply Earloop Mouth Cover 0r 25 PCS</t>
+  </si>
+  <si>
+    <t>10,000+ SOLDFAST SHIPPING✅BEST CHOICE Best PRICE</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/50-PCS-Face-Mask-Medical-Surgical-Disposable-3-Ply-Earloop-Mouth-Cover-0r-25-PCS/153950412320?hash=item23d828de20%3Ag%3A4G4AAOSw-XRez6V3&amp;LH_BIN=1</t>
+  </si>
+  <si>
     <t>KN95 Face Mask 5 Piece or 10 Piece Protective Respirator Covers Medical Grade</t>
   </si>
   <si>
@@ -123,15 +132,6 @@
     <t>https://www.ebay.com/itm/KN95-Face-Mask-5-Piece-or-10-Piece-Protective-Respirator-Covers-Medical-Grade/153936174294?hash=item23d74f9cd6%3Ag%3AA2gAAOSwAM5ewVJy&amp;LH_BIN=1</t>
   </si>
   <si>
-    <t>50 PCS Face Mask Medical Surgical Disposable 3-Ply Earloop Mouth Cover 0r 25 PCS</t>
-  </si>
-  <si>
-    <t>10,000+ SOLDFAST SHIPPING✅BEST CHOICE Best PRICE</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50-PCS-Face-Mask-Medical-Surgical-Disposable-3-Ply-Earloop-Mouth-Cover-0r-25-PCS/153950412320?hash=item23d828de20%3Ag%3A4G4AAOSw-XRez6V3&amp;LH_BIN=1</t>
-  </si>
-  <si>
     <t>KN95 5 Layer Medical Face Masks Mouth Covers Protective Respirator K N95</t>
   </si>
   <si>
@@ -144,6 +144,102 @@
     <t>https://www.ebay.com/itm/KN95-5-Layer-Medical-Face-Masks-Mouth-Covers-Protective-Respirator-K-N95/164202098239?hash=item263b352e3f%3Ag%3A9SwAAOSwDtReyyVl&amp;LH_BIN=1</t>
   </si>
   <si>
+    <t>50/100/500 Pcs Face Mask Level-2 Medical Surgical Disposable 3-Ply Mouth Cover</t>
+  </si>
+  <si>
+    <t>USA STOCK / / SHIP OUT WITHIN 1 BUSINESS DAY</t>
+  </si>
+  <si>
+    <t>$24.99 to $199.00</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/50-100-500-Pcs-Face-Mask-Level-2-Medical-Surgical-Disposable-3-Ply-Mouth-Cover/114273236024?hash=item1a9b373438%3Ag%3AaG0AAOSwywNfArjI&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>FDA Approved 3-Ply Disposable Blue Earloop Face Mask, Medical, Surgical, Dental</t>
+  </si>
+  <si>
+    <t>$10.95 to $44.95</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/FDA-Approved-3-Ply-Disposable-Blue-Earloop-Face-Mask-Medical-Surgical-Dental/362999738765?hash=item548478718d%3Ag%3A538AAOSw8G9eqal0&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>ASTM LEVEL 3 4-Ply Blue Disposable Medical Surgical Protection Filter Face Masks</t>
+  </si>
+  <si>
+    <t>In-Stock. Ships within 1 Business Day from Los Angeles</t>
+  </si>
+  <si>
+    <t>$59.99 to $114.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/ASTM-LEVEL-3-4-Ply-Blue-Disposable-Medical-Surgical-Protection-Filter-Face-Masks/164256973115?hash=item263e7a813b%3Ag%3AMb4AAOSwKule8Czf&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>Child Toddler Protective Surgical Face Mask Mouth Medical Disposable</t>
+  </si>
+  <si>
+    <t>Adult and Child 10 masks per pack discount for multiple</t>
+  </si>
+  <si>
+    <t>$9.99 to $12.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/Child-Toddler-Protective-Surgical-Face-Mask-Mouth-Medical-Disposable/224044608741?hash=item342a196ce5%3Ag%3Ai8QAAOSwQOpe5VrC&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>ASTM LEVEL 2 Blue Disposable Medical Surgical Protection Filter 3-Ply Face Masks</t>
+  </si>
+  <si>
+    <t>$39.99 to $74.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/ASTM-LEVEL-2-Blue-Disposable-Medical-Surgical-Protection-Filter-3-Ply-Face-Masks/164196642457?hash=item263ae1ee99%3Ag%3AY7UAAOSwgQZe9CHh&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>50/100/500 PCS Face Mask 3-Ply Disposable Medical Masks Mouth cover</t>
+  </si>
+  <si>
+    <t>✅CE APPROVED✅FAST SHIPPING✅HOSPITAL GRADE</t>
+  </si>
+  <si>
+    <t>$11.98 to $118.88</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/50-100-500-PCS-Face-Mask-3-Ply-Disposable-Medical-Masks-Mouth-cover/184291307047?hash=item2ae89e2e27%3Ag%3AqBsAAOSwQXdevJDh&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>10 / 20 / 50 Pack KN95 Face Mask Respirator Medical 5-Layer K N95 Protection</t>
+  </si>
+  <si>
+    <t>$8.99 to $109.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/10-20-50-Pack-KN95-Face-Mask-Respirator-Medical-5-Layer-K-N95-Protection/224033782509?hash=item3429743aed%3Ag%3AMX8AAOSwvpde9Pws&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>MEDICAL GRADE SURGICAL DISPOSABLE 3PLY FACE MASK</t>
+  </si>
+  <si>
+    <t>USA SELLER!!! SHIPS SAME DAY!!! QUICK DELIVERY!!</t>
+  </si>
+  <si>
+    <t>$22.99 to $729.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/MEDICAL-GRADE-SURGICAL-DISPOSABLE-3PLY-FACE-MASK/224051160591?hash=item342a7d660f%3Ag%3A6vgAAOSwd4pe7RYc&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>Medical Facemasks , Face Masks Social Distancing, Personal Protection CHOOSE QTY</t>
+  </si>
+  <si>
+    <t>$9.99 to $49.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/Medical-Facemasks-Face-Masks-Social-Distancing-Personal-Protection-CHOOSE-QTY/153931221790?hash=item23d7040b1e%3Ag%3AYCUAAOSwFdRevFrA&amp;LH_BIN=1</t>
+  </si>
+  <si>
     <t>50 PCS -Disposable Face Mask- Non Medical Surgical Mouth Nose Earloop Coverings</t>
   </si>
   <si>
@@ -156,163 +252,70 @@
     <t>https://www.ebay.com/itm/50-PCS-Disposable-Face-Mask-Non-Medical-Surgical-Mouth-Nose-Earloop-Coverings/143645635148?hash=item2171f2724c%3Ag%3AXQUAAOSw-ZFfBU9t&amp;LH_BIN=1</t>
   </si>
   <si>
-    <t>50/100/500 Pcs Face Mask Level-2 Medical Surgical Disposable 3-Ply Mouth Cover</t>
-  </si>
-  <si>
-    <t>USA STOCK / / SHIP OUT WITHIN 1 BUSINESS DAY</t>
-  </si>
-  <si>
-    <t>$24.99 to $199.00</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50-100-500-Pcs-Face-Mask-Level-2-Medical-Surgical-Disposable-3-Ply-Mouth-Cover/114273236024?hash=item1a9b373438%3Ag%3AaG0AAOSwywNfArjI&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>50/100/200 Protective Disposable Face Mask 3-Layer Medical C.E Approval FFP2</t>
+    <t>Disposable Face Mask Mouth Cover Medical Protective Respirator Masks K N95 KN95</t>
+  </si>
+  <si>
+    <t>$6.89 to $29.89</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/Disposable-Face-Mask-Mouth-Cover-Medical-Protective-Respirator-Masks-K-N95-KN95/114254222773?hash=item1a9a1515b5%3Ag%3At2EAAOSwV49e38Wq&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>3 PLY Face Mask Medical Surgical Dental Medical Cover Masks 5 10 or 20</t>
+  </si>
+  <si>
+    <t>In-Stock. Ships within 1 Business Day.</t>
+  </si>
+  <si>
+    <t>$8.99 to $29.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/3-PLY-Face-Mask-Medical-Surgical-Dental-Medical-Cover-Masks-5-10-or-20/164160367926?hash=item2638b86d36%3Ag%3AfsoAAOSwHt9elSyL&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>25-50 PCS TUORen Genuine Hospital Surgical Face Mask Medical Disposable 3-Ply</t>
+  </si>
+  <si>
+    <t>$24.99 to $44.99</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/25-50-PCS-TUORen-Genuine-Hospital-Surgical-Face-Mask-Medical-Disposable-3-Ply/392807533449?hash=item5b75274b89%3Ag%3AXNkAAOSwBSFeuKUu&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>50pk 3-Ply Surgical Style Non-Medical Face Mask OR 1pk 3M N95 Respirator OR KN95</t>
+  </si>
+  <si>
+    <t>See 3M N95 Models 07048-1805s-1860-1860s-8000-8200-8210</t>
+  </si>
+  <si>
+    <t>$3.99 to $7.95</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/50pk-3-Ply-Surgical-Style-Non-Medical-Face-Mask-OR-1pk-3M-N95-Respirator-OR-KN95/402323841978?hash=item5dac5ea3ba%3Ag%3AiKgAAOSwE4ZfCq7-&amp;LH_BIN=1</t>
+  </si>
+  <si>
+    <t>Protective Disposable Face Mask 3-Layers Medical C.E Approval FFP2 U.S Stocks</t>
   </si>
   <si>
     <t>" Orlando, FL Reputable Seller,In Stock Ship Same Day "</t>
   </si>
   <si>
-    <t>$11.88 to $199.00</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50-100-200-Protective-Disposable-Face-Mask-3-Layer-Medical-C-E-Approval-FFP2/233588946573?hash=item3662fc768d%3Ag%3A6qAAAOSw-RlevsD6&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>NEW LISTINGBYD DE2322 N95 Respirator Face Mask CE FDA NIOSH Approved Medical Use Fast Ship</t>
-  </si>
-  <si>
-    <t>* 20PCS/BOX * INDIVIDUALLY SEALED * IN-STOCK US *</t>
-  </si>
-  <si>
-    <t>$45.99 to $169.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/BYD-DE2322-N95-Respirator-Face-Mask-CE-FDA-NIOSH-Approved-Medical-Use-Fast-Ship/283948457562?hash=item421ca59e5a%3Ag%3AZXkAAOSwMYJfDmev&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>FDA Approved 3-Ply Disposable Blue Earloop Face Mask, Medical, Surgical, Dental</t>
-  </si>
-  <si>
-    <t>$10.95 to $44.95</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/FDA-Approved-3-Ply-Disposable-Blue-Earloop-Face-Mask-Medical-Surgical-Dental/362999738765?hash=item548478718d%3Ag%3A538AAOSw8G9eqal0&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>ASTM LEVEL 3 4-Ply Blue Disposable Medical Surgical Protection Filter Face Masks</t>
-  </si>
-  <si>
-    <t>In-Stock. Ships within 1 Business Day from Los Angeles</t>
-  </si>
-  <si>
-    <t>$59.99 to $114.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/ASTM-LEVEL-3-4-Ply-Blue-Disposable-Medical-Surgical-Protection-Filter-Face-Masks/164256973115?hash=item263e7a813b%3Ag%3AMb4AAOSwKule8Czf&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>50/100/500 PCS Face Mask 3-Ply Disposable Medical Masks Mouth cover</t>
-  </si>
-  <si>
-    <t>✅CE APPROVED✅FAST SHIPPING✅HOSPITAL GRADE</t>
-  </si>
-  <si>
-    <t>$11.98 to $118.88</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50-100-500-PCS-Face-Mask-3-Ply-Disposable-Medical-Masks-Mouth-cover/184291307047?hash=item2ae89e2e27%3Ag%3AqBsAAOSwQXdevJDh&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>ASTM LEVEL 2 Blue Disposable Medical Surgical Protection Filter 3-Ply Face Masks</t>
-  </si>
-  <si>
-    <t>$39.99 to $74.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/ASTM-LEVEL-2-Blue-Disposable-Medical-Surgical-Protection-Filter-3-Ply-Face-Masks/164196642457?hash=item263ae1ee99%3Ag%3AY7UAAOSwgQZe9CHh&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>MEDICAL GRADE SURGICAL DISPOSABLE 3PLY FACE MASK</t>
-  </si>
-  <si>
-    <t>USA SELLER!!! SHIPS SAME DAY!!! QUICK DELIVERY!!</t>
-  </si>
-  <si>
-    <t>$22.99 to $729.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/MEDICAL-GRADE-SURGICAL-DISPOSABLE-3PLY-FACE-MASK/224051160591?hash=item342a7d660f%3Ag%3A6vgAAOSwd4pe7RYc&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>Protective Disposable Face Mask 3-Layers Medical C.E Approval FFP2 U.S Stocks</t>
-  </si>
-  <si>
     <t>$11.92 to $218.00</t>
   </si>
   <si>
     <t>https://www.ebay.com/itm/Protective-Disposable-Face-Mask-3-Layers-Medical-C-E-Approval-FFP2-U-S-Stocks/333599602260?hash=item4dac15f654%3Ag%3AcCsAAOSwfWFe4PkQ&amp;LH_BIN=1</t>
   </si>
   <si>
-    <t>50pk 3-Ply Surgical Style Non-Medical Face Mask OR 1pk 3M N95 Respirator OR KN95</t>
-  </si>
-  <si>
-    <t>See 3M N95 Models 07048-1805s-1860-1860s-8000-8200-8210</t>
-  </si>
-  <si>
-    <t>$3.99 to $7.95</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/50pk-3-Ply-Surgical-Style-Non-Medical-Face-Mask-OR-1pk-3M-N95-Respirator-OR-KN95/402323841978?hash=item5dac5ea3ba%3Ag%3AiKgAAOSwE4ZfCq7-&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>Medical Facemasks , Face Masks Social Distancing, Personal Protection CHOOSE QTY</t>
-  </si>
-  <si>
-    <t>$9.99 to $49.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/Medical-Facemasks-Face-Masks-Social-Distancing-Personal-Protection-CHOOSE-QTY/153931221790?hash=item23d7040b1e%3Ag%3AYCUAAOSwFdRevFrA&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>3 PLY Face Mask Medical Surgical Dental Medical Cover Masks 5 10 or 20</t>
-  </si>
-  <si>
-    <t>In-Stock. Ships within 1 Business Day.</t>
-  </si>
-  <si>
-    <t>$8.99 to $29.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/3-PLY-Face-Mask-Medical-Surgical-Dental-Medical-Cover-Masks-5-10-or-20/164160367926?hash=item2638b86d36%3Ag%3AfsoAAOSwHt9elSyL&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>Disposable Face Mask Mouth Cover Medical Protective Respirator Masks K N95 KN95</t>
-  </si>
-  <si>
-    <t>$6.89 to $29.89</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/Disposable-Face-Mask-Mouth-Cover-Medical-Protective-Respirator-Masks-K-N95-KN95/114254222773?hash=item1a9a1515b5%3Ag%3At2EAAOSwV49e38Wq&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>10 PCS All Keeper KF94 Mask Made in Korea Surgical Medical FDA Approved Face</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/10-PCS-All-Keeper-KF94-Mask-Made-in-Korea-Surgical-Medical-FDA-Approved-Face/274423471661?_trkparms=ispr%3D1&amp;hash=item3fe4e9de2d%3Ag%3A2a4AAOSww%7E9fC8XO&amp;enc=AQAFAAACYBaobrjLl8XobRIiIML1V4Imu%2Fn%2BzU5L90Z278x5ickkY3FSd4Ad8xn3oRtkVexxrEAlzHw8Z2eTsBVcqVn%2BnTPe2YQ%2BqX7J3NAv7QjFqyXhXB%2FQfrRLbCa6ARGvtIQKkqgY91khHqBP2YYDsRkfozZ1cisq47uQRgYSni%2BLNaZ9oqPswtcMHqRYdpn6kD1ne9bWdoNITCp%2BDdcKKriFXmzbFcdgi6NLY09aJFvE9ZsqrZs1m1zDGVVAlDCeqeHLsNgVtd7e%2B4E0WSDUdx1wgci7isALyNe0n7bWpEcWWHEHNMvy7wJMA30fqjlYJfuHwv%2Fd5dRcio6o%2BJGOCQPKMBAYhqd4BHTpgQyj3LOYo1VMaSApAVxt7wKZJ6yB6HRuIYfpBUpxwkVx58xmLA0y2qn1UNCdxks2hgLJjAElQoyk0RCJZ2fRIXS0zzQ1%2BfQjrv%2BW7cmyHJynALLJKrUfCtZ8NxIG5daPsExTxbFHujFJK%2BkxdEXo6dPaVcjaywGUCA29U9FzSiwnRfN7RjMRi7Lmyy00k6I3PfzN2eFwhodgAGULFxkCYPBcMX%2BIG6EtIZze8Xobdxh096icANcfZ%2B%2FaZHctMF93NQNTeqT2DuSS%2F0ZGKjjefWa14mdF%2BlB0T3W7qUmp1k%2Fh3FjQx5ZcAdEQv2oYrpx4UFQmLQrPDmcznCwvbzwViz73YmK6dZ8W%2FV9kzx2eLjR41EIXM2NsHHpOprVQR6Mb8%2FSS79ZQm9fK0Y414tYcrdbWn9D3hyv8EulEKvkodnHq9bna9LVehF%2FKbTrWLvy%2FDzyHr4ercp7%2B&amp;checksum=274423471661080ec5151d0c47819dca4ec5deb5757f&amp;LH_BIN=1</t>
-  </si>
-  <si>
-    <t>Child Toddler Protective Surgical Face Mask Mouth Medical Disposable</t>
-  </si>
-  <si>
-    <t>Adult and Child 10 masks per pack discount for multiple</t>
-  </si>
-  <si>
-    <t>$9.99 to $12.99</t>
-  </si>
-  <si>
-    <t>https://www.ebay.com/itm/Child-Toddler-Protective-Surgical-Face-Mask-Mouth-Medical-Disposable/224044608741?_trkparms=ispr%3D1&amp;hash=item342a196ce5%3Ag%3Ai8QAAOSwQOpe5VrC&amp;enc=AQAFAAACYBaobrjLl8XobRIiIML1V4Imu%2Fn%2BzU5L90Z278x5ickkgCVySCgrNFPU8Iu85TabMEttovNUnnLDy7xu0FGMbjUiCxGatwSBEhIEHhIH1g3oQZCKoNcpbU7tiIw13JhBvvPCCpKfZjstJqGIlHK8ryI6qUj6ilyo%2B%2B352HzUutOL4LOVcI8qC1IdaKr22yX5Cnh1nzGQpqa%2FCYxWQjuMyxqce9y38VO4H6DlOI8Ppy4DgjDXuW5cxWr3EKVwUyKrR%2FNyCweRg5yypxfQx7DKL3onTGfF0FLKjAeNVkZzvIiMSJK063fz5qr05%2FzRTd0JHj5cDJ2HBdfvOjZGqqhcfKBq6EATBrBaHYR1DDozbgwlKKZabe2R4X6Bybt8sgGj6bLUqQcDMnQfMBCGFY5Fqgnlzy3ZMUzRa%2B9kFQy6nR1tyvCVT3K7lUFlWXJ1jz%2BjWvHgu9ZTZXr0cv9Z0UMdnSpTl7vjytyVds21%2FU292v4hcNB6vtSIzOBKDTO4WsYy1RE9xD%2FBARKOApCOwuVTAHAqs%2FouWenOlLxpnBKs%2FR2BRI5EL4LQBVJOb4vEPOJHTU0%2BA44LRHqshcRMpyKNCQ5IyCzkRATyYf9YEX5LxmrXo2ThRW%2FbkLnIVVjWMYOkOS8%2BGgo3vZgqSjKzpBXyA5BjPl8nlH9xNnBTEsVsOVG4fFx8xM4ypVnfPHH%2F27o3Z0yoFE4t0MZxYusTobO4%2B9OH5eNmLXk2pj9SxrChNF3NjJRroOyWDoi69y2Vn%2FPW7veKkEx%2FzkaHINscT%2BabKcC3W0yglhdwqGMQ2788uSw9&amp;checksum=224044608741080ec5151d0c47819dca4ec5deb5757f&amp;LH_BIN=1</t>
+    <t>ASTM LEVEL 2 Disposable Medical Surgical Filter Face Masks 3 Ply Blue, 50 or 100</t>
+  </si>
+  <si>
+    <t>BUY 5 GET 1 FREE</t>
+  </si>
+  <si>
+    <t>$61.95 to $112.50</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/ASTM-LEVEL-2-Disposable-Medical-Surgical-Filter-Face-Masks-3-Ply-Blue-50-or-100/174265987559?hash=item28930ff1e7%3Ag%3A9c0AAOSwNZNeqbIC&amp;LH_BIN=1</t>
   </si>
   <si>
     <t>Perfetta Ultra FDA CE Face Mask ASTM Level 3 4 Ply F2100 Type IIR Medical Use</t>
@@ -679,14 +682,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14C61236-475C-4B42-9011-022037BDE5EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B2A0125-3A06-4F53-8A9C-183D998DA037}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="71.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -802,25 +805,25 @@
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
         <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>31</v>
-      </c>
-      <c r="C8" s="1">
-        <v>15.99</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
@@ -868,271 +871,271 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
         <v>42</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
         <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>50</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
         <v>51</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
       </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
         <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
         <v>61</v>
-      </c>
-      <c r="C16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="s">
         <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>68</v>
-      </c>
-      <c r="C18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
         <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
         <v>74</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
         <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
         <v>81</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
         <v>82</v>
-      </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
         <v>85</v>
       </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
         <v>86</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
         <v>88</v>
       </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1">
-        <v>39.99</v>
+      <c r="C24" t="s">
+        <v>89</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B25" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>